<commit_message>
Add Patrick Malzan to COM results.
</commit_message>
<xml_diff>
--- a/2022/com-20220911.xlsx
+++ b/2022/com-20220911.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C298BF-800E-9A43-9C52-7C6C2074C801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731305E3-B7E3-9747-A8FD-67BD580EB4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="500" windowWidth="21660" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="91">
   <si>
     <t>class_index</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t xml:space="preserve"> DENNIS O'MEARA</t>
+  </si>
+  <si>
+    <t>SMF</t>
+  </si>
+  <si>
+    <t>PATRICK MALZAHN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1:04.626</t>
   </si>
 </sst>
 </file>
@@ -1157,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1405,6 +1414,17 @@
       </c>
       <c r="D32" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add results from final weekend. Fix up a couple classes in Met Council results.
</commit_message>
<xml_diff>
--- a/2022/com-20220911.xlsx
+++ b/2022/com-20220911.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731305E3-B7E3-9747-A8FD-67BD580EB4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4327685-6DB1-6E40-9384-1E4F1C12CB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="500" windowWidth="21660" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,18 +207,12 @@
     <t xml:space="preserve"> 1:06.469</t>
   </si>
   <si>
-    <t xml:space="preserve"> XS-A</t>
-  </si>
-  <si>
     <t xml:space="preserve"> DOUGLAS LINDMAN</t>
   </si>
   <si>
     <t xml:space="preserve"> 1:15.923 </t>
   </si>
   <si>
-    <t xml:space="preserve"> XS-B</t>
-  </si>
-  <si>
     <t xml:space="preserve"> BLAKE DOBLINGER</t>
   </si>
   <si>
@@ -295,6 +289,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 1:04.626</t>
+  </si>
+  <si>
+    <t>XA</t>
+  </si>
+  <si>
+    <t>XB</t>
   </si>
 </sst>
 </file>
@@ -1166,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1267,7 +1267,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -1388,7 +1388,7 @@
         <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
         <v>48</v>
@@ -1418,13 +1418,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
         <v>88</v>
-      </c>
-      <c r="C33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1451,128 +1451,128 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
         <v>61</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>62</v>
-      </c>
-      <c r="D38" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" t="s">
         <v>64</v>
       </c>
-      <c r="C40" t="s">
-        <v>65</v>
-      </c>
-      <c r="D40" t="s">
-        <v>66</v>
-      </c>
       <c r="E40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
         <v>67</v>
       </c>
-      <c r="B42" t="s">
+      <c r="E42" t="s">
         <v>68</v>
-      </c>
-      <c r="C42" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" t="s">
         <v>73</v>
-      </c>
-      <c r="C44" t="s">
-        <v>74</v>
-      </c>
-      <c r="E44" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
         <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
         <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" t="s">
         <v>81</v>
-      </c>
-      <c r="B49" t="s">
-        <v>73</v>
-      </c>
-      <c r="C49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E49" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>